<commit_message>
changes on Effective start date
</commit_message>
<xml_diff>
--- a/Server/Required_files/Available_NLP.xlsx
+++ b/Server/Required_files/Available_NLP.xlsx
@@ -618,9 +618,10 @@
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>{PersonNumber} STRICTL HAS TO BE 300008</t>
-        </is>
-      </c>
+          <t>{EffectiveStartDate} has to be less or equal to {EffectiveEndDate}</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
           <t>Venkataraman_Test_Worker.py</t>
@@ -672,7 +673,6 @@
           <t>must be less than {StartDate}</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
           <t>Venkataraman_Test_Worker.py</t>

</xml_diff>

<commit_message>
Issues logged with year 4712 is fixed with both passed dataframes and also with the populating of those values for all the empty effective end dates properly,
</commit_message>
<xml_diff>
--- a/Server/Required_files/Available_NLP.xlsx
+++ b/Server/Required_files/Available_NLP.xlsx
@@ -1,15 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
-  </bookViews>
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -21,7 +17,7 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -51,7 +47,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -166,7 +162,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,7 +197,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,20 +264,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -403,7 +395,46 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
@@ -414,18 +445,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="14.21875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="27.109375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="9.6640625" bestFit="1" customWidth="1" min="3" max="3"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -450,236 +476,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Suffix</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Suffix value must have Senior value, Suffix value must have Junior value, Suffix value must not be null or empty</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>OR, AND, AND</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
-        <is>
-          <t>Suffix.py</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Person Number</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>person name should always be an integer</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>AND</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Person_Number.py</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>FirstName</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>First Name should not have john</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>AND</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>FirstName.py</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Effective Start Date</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>effective start date must be latest from than 2000</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>AND</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Effective_Start_Date.py</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Preferred Name</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>preferred Name must only contain nAn or null values</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>AND</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Preferred_Name.py</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>PersonNumber</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>i want the {PersonNumber} to be unique</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
         <is>
           <t>Venkataraman_Test_Worker.py</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>EffectiveStartDate</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>{EffectiveStartDate} has to be above 1970</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Venkataraman_Test_Worker.py</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>LastName</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>cannot be numbers, cannot be fox</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>AND, AND</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>LastName.py</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>{EffectiveStartDate} has to be less or equal to {EffectiveEndDate}</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Venkataraman_Test_Worker.py</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Location Code</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Country must be US {Country}</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Location_Code.py</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>HourlySalariedCode</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">should not be empty or blank </t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>.py</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>DateOfBirth</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>must be less than {StartDate}</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Venkataraman_Test_Worker.py</t>
-        </is>
-      </c>
-    </row>
+    <row r="10"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>